<commit_message>
change file path to run regression
</commit_message>
<xml_diff>
--- a/04_regression/03_output/peak_point_reg_wage_age.xlsx
+++ b/04_regression/03_output/peak_point_reg_wage_age.xlsx
@@ -371,10 +371,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>42.45100213446527</v>
+        <v>42.0938145374306</v>
       </c>
       <c r="B2">
-        <v>6329.215377934609</v>
+        <v>6281.914324494228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix identation and turn some variables into factors
</commit_message>
<xml_diff>
--- a/04_regression/03_output/peak_point_reg_wage_age.xlsx
+++ b/04_regression/03_output/peak_point_reg_wage_age.xlsx
@@ -371,10 +371,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>42.0938145374306</v>
+        <v>42.07507574101696</v>
       </c>
       <c r="B2">
-        <v>6281.914324494228</v>
+        <v>6360.900765590047</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se ajusta la regresión y graficos
</commit_message>
<xml_diff>
--- a/04_regression/03_output/peak_point_reg_wage_age.xlsx
+++ b/04_regression/03_output/peak_point_reg_wage_age.xlsx
@@ -371,10 +371,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>42.07507574101696</v>
+        <v>41.84451055447188</v>
       </c>
       <c r="B2">
-        <v>6360.900765590047</v>
+        <v>6259.493667618731</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aplicación de boostrap en intervalos para cada salario predicho
</commit_message>
<xml_diff>
--- a/04_regression/03_output/peak_point_reg_wage_age.xlsx
+++ b/04_regression/03_output/peak_point_reg_wage_age.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,12 +360,22 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>age</t>
+          <t>peak_age</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>wage</t>
+          <t>peak_wage</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>ci_wage_lo</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ci_wage_hi</t>
         </is>
       </c>
     </row>
@@ -374,7 +384,13 @@
         <v>41.84451055447188</v>
       </c>
       <c r="B2">
-        <v>6259.493667618731</v>
+        <v>6259.493667603875</v>
+      </c>
+      <c r="C2">
+        <v>6133.368678375889</v>
+      </c>
+      <c r="D2">
+        <v>6389.226704294119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>